<commit_message>
:chart: CDN & mififier
</commit_message>
<xml_diff>
--- a/rapport.xlsx
+++ b/rapport.xlsx
@@ -1,9 +1,9 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24020"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{08BB6E21-341D-43A9-A4B5-1F24FA511396}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{D3D45F39-D446-4690-8F43-E799FFC446FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="54" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="60">
   <si>
     <t>Catégorie</t>
   </si>
@@ -58,21 +58,132 @@
     <t>https://www.w3.org/WAI/standards-guidelines/aria/</t>
   </si>
   <si>
+    <t>Typos dans la sémantique</t>
+  </si>
+  <si>
+    <t>Il est important de prêter attention à la sémantique HTML car cela permet aux lecteurs d'écrans de mieux s'orienter dans la page, de plus, une page bien organisée et agréable à lire incitera les gens à rester plus longtemps, ce qui fera à son tour grimper le référencement</t>
+  </si>
+  <si>
+    <t>Modification de détails : balise &lt;li&gt; inutile dans la nav, moins de div et plus de section, title sur icone réseaux sociaux...</t>
+  </si>
+  <si>
+    <t>https://www.nvda-fr.org/doc/keyCommands.html</t>
+  </si>
+  <si>
+    <t>Accessibilité/SEO</t>
+  </si>
+  <si>
+    <t>L'outils wave fait apparaître un certain nombre de problèmes</t>
+  </si>
+  <si>
+    <t>L'accessibilité est une des données prise en compte dans le rapport SEO de lighthouse. Par ailleurs, un mauvais score sur ce point rend le site inaccessible à une partie des usagers et fait donc perdre des clients potentiels</t>
+  </si>
+  <si>
+    <t>Améliorer les contrastes, ne pas mettre de textes sous forme d'image, augmenter la taille des textes trop petits, indiquer une langue pour l'ensemble de la page</t>
+  </si>
+  <si>
+    <t>https://wave.webaim.org/</t>
+  </si>
+  <si>
+    <t>SEO/Accessibilité</t>
+  </si>
+  <si>
+    <t>Format et taille des images inadaptés, alt incohérents</t>
+  </si>
+  <si>
+    <t>Le temps de chargement du site est négativement impacté par le format .bmp et la taille de certaines images, de plus des techniques dites "blackhat" sont utilisés sur l'attribut "alt" ce que l'algorithme de google pénalise, et cela complique le travail des lecteurs d'écran</t>
+  </si>
+  <si>
+    <t>Passer au format webp, retailler et/ou compresser les images, changer le texte des attributs alt</t>
+  </si>
+  <si>
+    <t>https://www.w3.org/WAI/test-evaluate/preliminary/#images &amp; https://www.seo.fr/blog/comprendre-le-black-hat-seo</t>
+  </si>
+  <si>
     <t>SEO</t>
   </si>
   <si>
+    <t>Pas de CDN ni de fichiers minifiés</t>
+  </si>
+  <si>
+    <t>Minifier les fichiers et utiliser des CDN permet de ralentir le temps de chargement de la page</t>
+  </si>
+  <si>
+    <t>minifier les fichiers quand c'est possible (fichiers css...) et utiliser un CDN quand ce n'est pas le cas (gmaps, jquery.touchSwipe...)</t>
+  </si>
+  <si>
+    <t>https://www.sitepoint.com/7-reasons-to-use-a-cdn/</t>
+  </si>
+  <si>
+    <t>gmaps.js est chargé par le site mais pas utilisé</t>
+  </si>
+  <si>
+    <t>Il faut soit utiliser cette dependencie, soit la supprimer car son chargement ralentit inutilement l'affichage du site</t>
+  </si>
+  <si>
+    <t>En attendant une décision finale, affichage d'un plan en utilisant un iframe</t>
+  </si>
+  <si>
+    <t>Dependencies pas à jour</t>
+  </si>
+  <si>
+    <t>Bootstrap et Jquery ne sont pas à jour, ce qui crée des vulnérabilités en terme de sécurités</t>
+  </si>
+  <si>
+    <t>Mettre à jour les dependecies</t>
+  </si>
+  <si>
+    <t>https://developers.google.com/web/tools/lighthouse#devtools</t>
+  </si>
+  <si>
     <t>Problèmes de UX design</t>
   </si>
   <si>
     <t>L'apparence de l'interface utilisateur influe sur son expérience et a un impact direct sur le temps qu'il va passer sur le site ce qui a son tour a un impact sur le référencement par les crawlers</t>
   </si>
   <si>
-    <t>Faire une navigation et des titres visibles et accessibles,  améliorer le visuel (centrer les &lt; &gt; + sur les images...)</t>
+    <t>Faire une navigation et des titres visibles et accessibles,  améliorer le visuel (centrer les &lt; &gt; + sur les images, un espace en trop, rajout d'un accent sur une majuscule (code html)...)</t>
   </si>
   <si>
     <t>https://www.matthieu-tranvan.fr/referencement-naturel/checklist-seo-25-bonnes-pratiques-on-site-pour-renforcer-votre-referencement-naturel.html#L%E2%80%99experience_utilisateur_a_aussi_un_impact_SEO</t>
   </si>
   <si>
+    <t>Pas de fichier robots.txt / sitemap</t>
+  </si>
+  <si>
+    <t>Les fichiers robots.txt et sitemap permettent un meilleur référencement par les crawlers</t>
+  </si>
+  <si>
+    <t>Ajouter un fichier robots.txt et un fichier sitemap</t>
+  </si>
+  <si>
+    <t>https://www.anthedesign.fr/referencement/fichier-robots-txt/ &amp; https://www.sitemaps.org/PROTOCOL.html</t>
+  </si>
+  <si>
+    <t>Pas de formatage des données avec schema.org</t>
+  </si>
+  <si>
+    <t>Les micro-datas facilitent le travail des crawlers, ce qui est récompensé par l'algorithme des moteurs de recherche</t>
+  </si>
+  <si>
+    <t>Formater les informations sur la page du formulaire de contact</t>
+  </si>
+  <si>
+    <t>https://schema.org/LocalBusiness</t>
+  </si>
+  <si>
+    <t>Des erreurs CSS et HTML apparaissent au validateur du W3C</t>
+  </si>
+  <si>
+    <t>Un code bien conçu a un impact sur l'accessibilité et le SEO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Supression de code deprecated (balise keyword, font-smooth...) </t>
+  </si>
+  <si>
+    <t>https://validator.w3.org/</t>
+  </si>
+  <si>
     <t>Absence de google analytics</t>
   </si>
   <si>
@@ -85,98 +196,23 @@
     <t>https://marketingplatform.google.com/intl/fr/about/analytics/benefits/</t>
   </si>
   <si>
-    <t>Accessibilité/SEO</t>
-  </si>
-  <si>
-    <t>L'outils wave fait apparaître un certain nombre de problèmes</t>
-  </si>
-  <si>
-    <t>L'accessibilité est une des données prise en compte dans le rapport SEO de lighthouse. Par ailleurs, un mauvais score sur ce point rend le site inaccessible à une partie des usagers et fait donc perdre des clients potentiels</t>
-  </si>
-  <si>
-    <t>Améliorer les contrastes, ne pas mettre de textes sous forme d'image, augmenter la taille des textes trop petits, indiquer une langue pour l'ensemble de la page</t>
-  </si>
-  <si>
-    <t>https://wave.webaim.org/</t>
-  </si>
-  <si>
-    <t>Dependencies pas à jour</t>
-  </si>
-  <si>
-    <t>Bootstrap et Jquery ne sont pas à jour, ce qui crée des vulnérabilités en terme de sécurités</t>
-  </si>
-  <si>
-    <t>Mettre à jour les dependecies</t>
-  </si>
-  <si>
-    <t>https://developers.google.com/web/tools/lighthouse#devtools</t>
-  </si>
-  <si>
-    <t>Pas de fichier robots.txt / sitemap</t>
-  </si>
-  <si>
-    <t>Les fichiers robots.txt et sitemap permettent un meilleur référencement par les crawlers</t>
-  </si>
-  <si>
-    <t>Ajouter un fichier robots.txt et un fichier sitemap</t>
-  </si>
-  <si>
-    <t>https://www.anthedesign.fr/referencement/fichier-robots-txt/ &amp; https://www.sitemaps.org/PROTOCOL.html</t>
-  </si>
-  <si>
-    <t>SEO/Accessibilité</t>
-  </si>
-  <si>
-    <t>Format et taille des images inadaptés, alt incohérents</t>
-  </si>
-  <si>
-    <t>Le temps de chargement du site est négativement impacté par le format .bmp et la taille de certaines images, de plus des techniques dites "blackhat" sont utilisés sur l'attribut "alt" ce que l'algorithme de google pénalise, et cela complique le travail des lecteurs d'écran</t>
-  </si>
-  <si>
-    <t>Passer au format webp, retailler et/ou compresser les images, changer le texte des attributs alt</t>
-  </si>
-  <si>
-    <t>https://www.w3.org/WAI/test-evaluate/preliminary/#images &amp; https://www.seo.fr/blog/comprendre-le-black-hat-seo</t>
-  </si>
-  <si>
-    <t>Pas de formatage des données avec schema.org</t>
-  </si>
-  <si>
-    <t>Les micro-datas facilitent le travail des crawlers, ce qui est récompensé par l'algorithme des moteurs de recherche</t>
-  </si>
-  <si>
-    <t>Formater les informations sur la page du formulaire de contact</t>
-  </si>
-  <si>
-    <t>https://schema.org/LocalBusiness</t>
-  </si>
-  <si>
-    <t>Des erreurs CSS et HTML apparaissent au validateur du W3C</t>
-  </si>
-  <si>
-    <t>Un code bien conçu a un impact sur l'accessibilité et le SEO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Supression de code deprecated (balise keyword, font-smooth...) </t>
-  </si>
-  <si>
-    <t>https://validator.w3.org/</t>
-  </si>
-  <si>
-    <t>gmaps.js est chargé par le site mais pas utilisé</t>
-  </si>
-  <si>
-    <t>Il faut soit utiliser cette dependencie, soit la supprimer car son chargement ralentit inutilement l'affichage du site</t>
-  </si>
-  <si>
-    <t>En attendant une décision finale, affichage d'un plan en utilisant un iframe</t>
+    <t>mis gmaps sur form contact en cdn</t>
+  </si>
+  <si>
+    <t>jqBootstrapValidation (plugin bootstrap pour form)</t>
+  </si>
+  <si>
+    <t>sur les 2 pages : jquery.touchSwipe (plugin pour tel pour le tactile)</t>
+  </si>
+  <si>
+    <t>semantique : balise li nav inutile, moins de div, espace en trop, manquait un accent (code html), title sur icone réseaux sociaux</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +239,12 @@
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFD4D4D4"/>
+      <name val="Consolas"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -232,14 +274,17 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -557,10 +602,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E12"/>
+  <dimension ref="A1:E32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -604,24 +649,24 @@
     </row>
     <row r="3" spans="1:5">
       <c r="A3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="C3" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="D3" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>13</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>14</v>
       </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" s="2" t="s">
-        <v>10</v>
+        <v>14</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>15</v>
@@ -655,120 +700,173 @@
     </row>
     <row r="6" spans="1:5">
       <c r="A6" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="E6" s="3" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="E7" s="3" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="2" t="s">
         <v>33</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="2" t="s">
         <v>34</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>35</v>
-      </c>
-      <c r="E8" s="3" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B9" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C9" s="2" t="s">
         <v>37</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="E9" s="3" t="s">
+    </row>
+    <row r="10" spans="1:5">
+      <c r="A10" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="2" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" ht="28.5" customHeight="1">
-      <c r="A10" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="2" t="s">
+      <c r="C10" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="C10" s="2" t="s">
+      <c r="D10" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="D10" s="4" t="s">
+      <c r="E10" s="3" t="s">
         <v>43</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>44</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" s="2" t="s">
-        <v>10</v>
+        <v>24</v>
       </c>
       <c r="B11" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="C11" s="2" t="s">
         <v>45</v>
       </c>
-      <c r="C11" s="2" t="s">
+      <c r="D11" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="D11" s="2" t="s">
+      <c r="E11" s="3" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="12" spans="1:5">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5">
+      <c r="A13" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="28" spans="1:1" ht="30">
+      <c r="A28" s="4" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="29" spans="1:1" ht="45">
+      <c r="A29" s="4" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="30" spans="1:1" ht="45">
+      <c r="A30" s="4" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="31" spans="1:1">
+      <c r="A31" s="5"/>
+    </row>
+    <row r="32" spans="1:1" ht="90">
+      <c r="A32" s="4" t="s">
+        <v>59</v>
+      </c>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="E2" r:id="rId1" xr:uid="{43730EC0-AAA3-4DC8-939B-6F041B86E113}"/>
-    <hyperlink ref="E3" r:id="rId2" location="L%E2%80%99experience_utilisateur_a_aussi_un_impact_SEO" xr:uid="{F2807259-5AF7-435F-A848-57FF79D5A2E6}"/>
-    <hyperlink ref="E4" r:id="rId3" xr:uid="{2A1BDE5A-8B80-4D89-B43F-83C35E8480F7}"/>
-    <hyperlink ref="E5" r:id="rId4" xr:uid="{285FE21E-E497-4F12-AEB6-FAC64AF08A78}"/>
-    <hyperlink ref="E6" r:id="rId5" location="devtools" xr:uid="{C784C991-7229-4788-97A4-AE764AE69207}"/>
-    <hyperlink ref="E7" r:id="rId6" xr:uid="{389A8AC3-1D12-4F03-ACF7-250B5C887796}"/>
-    <hyperlink ref="E8" r:id="rId7" location="images &amp; https://www.seo.fr/blog/comprendre-le-black-hat-seo" xr:uid="{DF18DA75-BE5A-4E89-A955-365C6FC4F96A}"/>
-    <hyperlink ref="E9" r:id="rId8" xr:uid="{DDC455FA-F18D-4A0A-847D-8BA507490684}"/>
-    <hyperlink ref="E10" r:id="rId9" xr:uid="{EA7174EA-77DD-40C4-B2B1-4D954EEAC484}"/>
+    <hyperlink ref="E9" r:id="rId2" location="L%E2%80%99experience_utilisateur_a_aussi_un_impact_SEO" xr:uid="{F2807259-5AF7-435F-A848-57FF79D5A2E6}"/>
+    <hyperlink ref="E13" r:id="rId3" xr:uid="{2A1BDE5A-8B80-4D89-B43F-83C35E8480F7}"/>
+    <hyperlink ref="E4" r:id="rId4" xr:uid="{285FE21E-E497-4F12-AEB6-FAC64AF08A78}"/>
+    <hyperlink ref="E8" r:id="rId5" location="devtools" xr:uid="{C784C991-7229-4788-97A4-AE764AE69207}"/>
+    <hyperlink ref="E10" r:id="rId6" xr:uid="{389A8AC3-1D12-4F03-ACF7-250B5C887796}"/>
+    <hyperlink ref="E5" r:id="rId7" location="images &amp; https://www.seo.fr/blog/comprendre-le-black-hat-seo" xr:uid="{DF18DA75-BE5A-4E89-A955-365C6FC4F96A}"/>
+    <hyperlink ref="E11" r:id="rId8" xr:uid="{DDC455FA-F18D-4A0A-847D-8BA507490684}"/>
+    <hyperlink ref="E12" r:id="rId9" xr:uid="{EA7174EA-77DD-40C4-B2B1-4D954EEAC484}"/>
+    <hyperlink ref="E3" r:id="rId10" xr:uid="{2D905255-F06C-4B1D-AEC6-EDE2EFAC6EB5}"/>
+    <hyperlink ref="E6" r:id="rId11" xr:uid="{1501C555-4121-4DA9-BAFB-45A855CB9396}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>